<commit_message>
balance check after 1st p-score matching
</commit_message>
<xml_diff>
--- a/out/t1.xlsx
+++ b/out/t1.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="t0" sheetId="1" r:id="rId1"/>
+    <sheet name="t1_pre" sheetId="1" r:id="rId1"/>
+    <sheet name="t1_post" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -967,4 +968,664 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>var</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ctrl.mean/n</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ctrl.sd/%</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>ONE.mean/n</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ONE.sd/%</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>p.val</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>n</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>302</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>151</t>
+        </is>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>index</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2017-05-08</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>203.07</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2018-10-15</t>
+        </is>
+      </c>
+      <c r="F3">
+        <v>41.54</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>male</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>31.1</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="F4">
+        <v>31.8</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>0.971</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>age</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>43.28</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>10.57</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>42.72</t>
+        </is>
+      </c>
+      <c r="F5">
+        <v>11.11</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>0.610</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>unempl</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>4.23</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>0.11</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>3.82</t>
+        </is>
+      </c>
+      <c r="F6">
+        <v>0.04</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>b_46</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>6.6</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="F7">
+        <v>8.6</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>0.565</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>b_47</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>9.9</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="F8">
+        <v>13.2</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>0.367</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>b_84</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>6.6</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="F9">
+        <v>7.9</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>0.746</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>b_85</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>14.2</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="F10">
+        <v>13.9</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>b_86</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>5.6</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>0.596</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>b_87</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>26</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>8.6</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="F12">
+        <v>8.6</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>b_88</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>14.9</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="F13">
+        <v>14.6</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>1.000</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>b_99</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>6.6</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>0.946</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>y_none</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>73.97</t>
+        </is>
+      </c>
+      <c r="D15">
+        <v>26.29</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>71.69</t>
+        </is>
+      </c>
+      <c r="F15">
+        <v>28.07</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>0.392</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>y_dgp</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>7.92</t>
+        </is>
+      </c>
+      <c r="D16">
+        <v>17.44</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>8.99</t>
+        </is>
+      </c>
+      <c r="F16">
+        <v>19.41</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>0.974</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>y_edu</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>0.82</t>
+        </is>
+      </c>
+      <c r="D17">
+        <v>5.62</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0.83</t>
+        </is>
+      </c>
+      <c r="F17">
+        <v>4.68</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>0.723</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>y_sgdp</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>15.39</t>
+        </is>
+      </c>
+      <c r="D18">
+        <v>11.17</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>16.54</t>
+        </is>
+      </c>
+      <c r="F18">
+        <v>10.55</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>0.022</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>y_baby</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>3.19</t>
+        </is>
+      </c>
+      <c r="D19">
+        <v>11.86</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>3.26</t>
+        </is>
+      </c>
+      <c r="F19">
+        <v>12.2</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>0.689</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>y_flex</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>0.53</t>
+        </is>
+      </c>
+      <c r="D20">
+        <v>6.05</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0.53</t>
+        </is>
+      </c>
+      <c r="F20">
+        <v>6.51</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>0.730</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>y_cash</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
+      <c r="D21">
+        <v>3.22</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0.50</t>
+        </is>
+      </c>
+      <c r="F21">
+        <v>3.67</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>0.650</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>y_reval</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0.00</t>
+        </is>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>NaN</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>